<commit_message>
[Add] apparatus list in common folder
</commit_message>
<xml_diff>
--- a/common/ApparatusList.xlsx
+++ b/common/ApparatusList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70318E8-2AC4-4EF5-AD74-16B64FA6960F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4295EF-03CA-4AF9-84B7-1CD60B482E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="液液抽出" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="134">
   <si>
     <t>URL</t>
     <phoneticPr fontId="2"/>
@@ -657,6 +657,13 @@
   </si>
   <si>
     <t>https://axel.as-1.co.jp/asone/d/65-6891-76/</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>非表示にしました</t>
+    <rPh sb="0" eb="3">
+      <t>ヒヒョウジ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1036,7 +1043,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1102,15 +1109,15 @@
       <c r="D3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="1">
-        <v>24765</v>
+      <c r="E3" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="1" t="e">
         <f>E3*F3</f>
-        <v>24765</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>65</v>
@@ -1129,15 +1136,13 @@
       <c r="D4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="1">
-        <v>26854</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1">
         <v>1</v>
       </c>
       <c r="G4" s="1">
         <f>E4*F4</f>
-        <v>26854</v>
+        <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>70</v>
@@ -1166,15 +1171,13 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1">
-        <v>170</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>3</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ref="G6:G22" si="0">E6*F6</f>
-        <v>510</v>
+        <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>13</v>
@@ -1193,15 +1196,13 @@
       <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="1">
-        <v>2950</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>3</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>8850</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>17</v>
@@ -1220,15 +1221,13 @@
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1">
-        <v>220</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>2</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>440</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>20</v>
@@ -1247,15 +1246,13 @@
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="1">
-        <v>40</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>4</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>21</v>
@@ -1274,15 +1271,13 @@
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1">
-        <v>700</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>23</v>
@@ -1301,15 +1296,13 @@
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="1">
-        <v>330</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>26</v>
@@ -1328,15 +1321,13 @@
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="1">
-        <v>300</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
@@ -1355,15 +1346,13 @@
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1">
-        <v>140</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>2</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>33</v>
@@ -1382,15 +1371,13 @@
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="1">
-        <v>10</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1">
         <v>15</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>35</v>
@@ -1409,15 +1396,13 @@
       <c r="D15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="1">
-        <v>150</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="0"/>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>36</v>
@@ -1436,15 +1421,13 @@
       <c r="D16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="1">
-        <v>9200</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1">
         <v>2</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="0"/>
-        <v>18400</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>50</v>
@@ -1463,15 +1446,13 @@
       <c r="D17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="1">
-        <v>800</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1">
         <v>2</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>55</v>
@@ -1490,15 +1471,13 @@
       <c r="D18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="1">
-        <v>1250</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="1">
         <v>2</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>58</v>
@@ -1517,15 +1496,13 @@
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1">
-        <v>250</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1">
         <v>1</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>61</v>
@@ -1544,15 +1521,13 @@
       <c r="D20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="1">
-        <v>780</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1">
         <v>3</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="0"/>
-        <v>2340</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>62</v>
@@ -1571,15 +1546,13 @@
       <c r="D21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="1">
-        <v>2926</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="0"/>
-        <v>2926</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>30</v>
@@ -1598,15 +1571,13 @@
       <c r="D22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="1">
-        <v>4719</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1">
         <v>10</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="0"/>
-        <v>47190</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>97</v>
@@ -1635,15 +1606,13 @@
       <c r="D24" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="1">
-        <v>2178</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="G24" s="1">
         <f>E24*F24</f>
-        <v>2178</v>
+        <v>0</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>76</v>
@@ -1662,15 +1631,13 @@
       <c r="D25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="1">
-        <v>5957</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="1">
         <v>2</v>
       </c>
       <c r="G25" s="1">
         <f>E25*F25</f>
-        <v>11914</v>
+        <v>0</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>81</v>
@@ -1689,16 +1656,13 @@
       <c r="D26" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="1">
-        <f>26600*1.1</f>
-        <v>29260.000000000004</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="G26" s="1">
         <f>E26*F26</f>
-        <v>29260.000000000004</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>86</v>
@@ -1717,15 +1681,13 @@
       <c r="D27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="1">
-        <v>1804</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1">
         <v>1</v>
       </c>
       <c r="G27" s="1">
         <f>E27*F27</f>
-        <v>1804</v>
+        <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>90</v>
@@ -1744,15 +1706,13 @@
       <c r="D28" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="1">
-        <v>241</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="1">
         <v>1</v>
       </c>
       <c r="G28" s="1">
         <f>E28*F28</f>
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>93</v>
@@ -1781,15 +1741,13 @@
       <c r="D30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E30" s="1">
-        <v>10989</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="1">
         <v>1</v>
       </c>
       <c r="G30" s="1">
         <f>E30*F30</f>
-        <v>10989</v>
+        <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>130</v>
@@ -1808,15 +1766,13 @@
       <c r="D31" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E31" s="1">
-        <v>7469</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1">
         <v>1</v>
       </c>
       <c r="G31" s="1">
         <f>E31*F31</f>
-        <v>7469</v>
+        <v>0</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>104</v>
@@ -1835,15 +1791,13 @@
       <c r="D32" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="1">
-        <v>2992</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1">
         <v>1</v>
       </c>
       <c r="G32" s="1">
         <f>E32*F32</f>
-        <v>2992</v>
+        <v>0</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>106</v>
@@ -1862,15 +1816,13 @@
       <c r="D33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="1">
-        <v>3397</v>
-      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="1">
         <v>1</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" ref="G33:G38" si="1">E33*F33</f>
-        <v>3397</v>
+        <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>113</v>
@@ -1889,15 +1841,13 @@
       <c r="D34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="1">
-        <v>4389</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1">
         <v>4</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="1"/>
-        <v>17556</v>
+        <v>0</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>131</v>
@@ -1916,15 +1866,13 @@
       <c r="D35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="1">
-        <v>2540</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="1">
         <f t="shared" si="1"/>
-        <v>2540</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>120</v>
@@ -1943,15 +1891,13 @@
       <c r="D36" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="1">
-        <v>2822</v>
-      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="1">
         <v>8</v>
       </c>
       <c r="G36" s="1">
         <f t="shared" si="1"/>
-        <v>22576</v>
+        <v>0</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>132</v>
@@ -1970,15 +1916,13 @@
       <c r="D37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="1">
-        <v>5555</v>
-      </c>
+      <c r="E37" s="1"/>
       <c r="F37" s="1">
         <v>1</v>
       </c>
       <c r="G37" s="1">
         <f t="shared" si="1"/>
-        <v>5555</v>
+        <v>0</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>129</v>
@@ -1997,15 +1941,13 @@
       <c r="D38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="1">
-        <v>4444</v>
-      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="1">
         <v>1</v>
       </c>
       <c r="G38" s="1">
         <f t="shared" si="1"/>
-        <v>4444</v>
+        <v>0</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
change in apparatsu list
</commit_message>
<xml_diff>
--- a/common/ApparatusList.xlsx
+++ b/common/ApparatusList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4295EF-03CA-4AF9-84B7-1CD60B482E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3A5AA7-39B4-45FB-AF44-A0AB6469CD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="液液抽出" sheetId="2" r:id="rId1"/>
@@ -1043,7 +1043,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
[Change] added item to apparatus
</commit_message>
<xml_diff>
--- a/common/ApparatusList.xlsx
+++ b/common/ApparatusList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3A5AA7-39B4-45FB-AF44-A0AB6469CD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7AEED5-C8ED-4462-9AE5-F69BF034EF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="液液抽出" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="135">
   <si>
     <t>URL</t>
     <phoneticPr fontId="2"/>
@@ -623,31 +623,6 @@
     <t>65-6891-76</t>
   </si>
   <si>
-    <t>フィッティング 1/8" 10個入　9771</t>
-  </si>
-  <si>
-    <t>65-6691-72</t>
-  </si>
-  <si>
-    <t>フラットシールフェラル 1/8" 10個入 9774</t>
-    <rPh sb="19" eb="20">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>イ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>65-6691-75</t>
-  </si>
-  <si>
-    <t>https://axel.as-1.co.jp/asone/d/65-6691-75/</t>
-  </si>
-  <si>
-    <t>https://axel.as-1.co.jp/asone/d/65-6691-72/</t>
-  </si>
-  <si>
     <t>https://www.monotaro.com/p/3352/7794/</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -665,6 +640,27 @@
       <t>ヒヒョウジ</t>
     </rPh>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ブレッドボード・ジャンパーワイヤ(オス-メス) 15cm(赤)</t>
+  </si>
+  <si>
+    <t>DG01032-0024-WH-015</t>
+  </si>
+  <si>
+    <t>秋月電子通商</t>
+  </si>
+  <si>
+    <t>https://akizukidenshi.com/catalog/g/g108933/</t>
+  </si>
+  <si>
+    <t>ブレッドボード・ジャンパー延長ワイヤ(メス-メス) 15cm赤</t>
+  </si>
+  <si>
+    <t>0116-71905-01-015</t>
+  </si>
+  <si>
+    <t>https://akizukidenshi.com/catalog/g/g103474/</t>
   </si>
 </sst>
 </file>
@@ -674,7 +670,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -713,6 +709,21 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -738,7 +749,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -758,6 +769,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -1040,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C311BC-1417-4A6C-9D84-8A6A304F40E2}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1110,7 +1125,7 @@
         <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -1750,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
@@ -1821,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" ref="G33:G38" si="1">E33*F33</f>
+        <f t="shared" ref="G33:G36" si="1">E33*F33</f>
         <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -1850,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
@@ -1900,57 +1915,57 @@
         <v>0</v>
       </c>
       <c r="H36" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="1">
+        <v>108935</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A37" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="1">
-        <v>9771</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B38" s="1">
-        <v>9774</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>128</v>
+      <c r="B39" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="1">
+        <v>103474</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>